<commit_message>
Day 4 C# Day1 Documents
</commit_message>
<xml_diff>
--- a/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
+++ b/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\WiproBatch-25April\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5644AFD-0B5E-4879-885C-9214B8C43D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A22D7A-E27D-4DDA-A8FE-FC918882140C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="1" xr2:uid="{A334C00E-DF14-8E42-AC33-43AB2B07B0C8}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{A334C00E-DF14-8E42-AC33-43AB2B07B0C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1-schedule" sheetId="55" r:id="rId1"/>
@@ -2067,7 +2067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2171,32 +2171,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -2207,14 +2234,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2225,89 +2252,53 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2706,8 +2697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BDF0E5-7E6E-4AF4-9B24-6563F83F938C}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:F49"/>
+    <sheetView topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2725,16 +2716,16 @@
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="9" t="s">
@@ -2753,13 +2744,13 @@
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
@@ -2774,187 +2765,187 @@
       <c r="A5" s="15">
         <v>1</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="67" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A6" s="37">
+      <c r="A6" s="48">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="56"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A7" s="38"/>
-      <c r="B7" s="46" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="46"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A8" s="38"/>
-      <c r="B8" s="46" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="46"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A9" s="38"/>
-      <c r="B9" s="46" t="s">
+      <c r="A9" s="49"/>
+      <c r="B9" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="46"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A10" s="38"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="55" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A11" s="38"/>
-      <c r="B11" s="62" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="56"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="46"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A12" s="39"/>
-      <c r="B12" s="62" t="s">
+      <c r="A12" s="53"/>
+      <c r="B12" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="56"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A13" s="37">
+      <c r="A13" s="48">
         <v>1.2</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="56"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="46"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A14" s="38"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="49"/>
+      <c r="B14" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="46"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A15" s="38"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="49"/>
+      <c r="B15" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="46"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A16" s="39"/>
-      <c r="B16" s="46" t="s">
+      <c r="A16" s="53"/>
+      <c r="B16" s="55" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A17" s="37">
+      <c r="A17" s="48">
         <v>1.3</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="56"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="46"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A18" s="38"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="34" t="s">
         <v>187</v>
       </c>
@@ -2962,12 +2953,12 @@
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
       <c r="F18" s="36"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="56"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="46"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A19" s="38"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="26" t="s">
         <v>188</v>
       </c>
@@ -2975,318 +2966,318 @@
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="56"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="46"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A20" s="37">
+      <c r="A20" s="48">
         <v>1.4</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="56"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="46"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A21" s="38"/>
-      <c r="B21" s="46" t="s">
+      <c r="A21" s="49"/>
+      <c r="B21" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="46"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A22" s="38"/>
-      <c r="B22" s="46" t="s">
+      <c r="A22" s="49"/>
+      <c r="B22" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="39"/>
-      <c r="B23" s="46" t="s">
+      <c r="A23" s="53"/>
+      <c r="B23" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="46"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A24" s="37">
+      <c r="A24" s="48">
         <v>1.5</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="56"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="46"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A25" s="38"/>
-      <c r="B25" s="46" t="s">
+      <c r="A25" s="49"/>
+      <c r="B25" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="46"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A26" s="38"/>
-      <c r="B26" s="46" t="s">
+      <c r="A26" s="49"/>
+      <c r="B26" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="46"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A27" s="39"/>
-      <c r="B27" s="46" t="s">
+      <c r="A27" s="53"/>
+      <c r="B27" s="55" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="57"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" s="15">
         <v>2</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52" t="s">
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="H28" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="I28" s="55">
+      <c r="I28" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A29" s="37">
+      <c r="A29" s="48">
         <v>2.1</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="56"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A30" s="38"/>
-      <c r="B30" s="46" t="s">
+      <c r="A30" s="49"/>
+      <c r="B30" s="55" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A31" s="38"/>
-      <c r="B31" s="46" t="s">
+      <c r="A31" s="49"/>
+      <c r="B31" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A32" s="39"/>
-      <c r="B32" s="46" t="s">
+      <c r="A32" s="53"/>
+      <c r="B32" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A33" s="37">
+      <c r="A33" s="48">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="56"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A34" s="38"/>
-      <c r="B34" s="46" t="s">
+      <c r="A34" s="49"/>
+      <c r="B34" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A35" s="38"/>
-      <c r="B35" s="46" t="s">
+      <c r="A35" s="49"/>
+      <c r="B35" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="46"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A36" s="39"/>
-      <c r="B36" s="46" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="46"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A37" s="37">
+      <c r="A37" s="48">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="56"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="46"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A38" s="38"/>
-      <c r="B38" s="46" t="s">
+      <c r="A38" s="49"/>
+      <c r="B38" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A39" s="38"/>
-      <c r="B39" s="46" t="s">
+      <c r="A39" s="49"/>
+      <c r="B39" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="46"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A40" s="39"/>
-      <c r="B40" s="46" t="s">
+      <c r="A40" s="53"/>
+      <c r="B40" s="55" t="s">
         <v>211</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="46"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A41" s="37">
+      <c r="A41" s="48">
         <v>2.4</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="56"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A42" s="38"/>
+      <c r="A42" s="49"/>
       <c r="B42" s="34" t="s">
         <v>213</v>
       </c>
@@ -3294,12 +3285,12 @@
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
       <c r="F42" s="36"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="56"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="46"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A43" s="39"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="34" t="s">
         <v>214</v>
       </c>
@@ -3307,27 +3298,27 @@
       <c r="D43" s="35"/>
       <c r="E43" s="35"/>
       <c r="F43" s="36"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="56"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="46"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A44" s="37">
+      <c r="A44" s="48">
         <v>2.5</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="56"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="46"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A45" s="38"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="34" t="s">
         <v>216</v>
       </c>
@@ -3335,110 +3326,91 @@
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
       <c r="F45" s="36"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="56"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="46"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A46" s="39"/>
-      <c r="B46" s="26" t="s">
+      <c r="A46" s="53"/>
+      <c r="B46" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="56"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="46"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A47" s="37">
+      <c r="A47" s="48">
         <v>2.6</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="56"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="46"/>
     </row>
     <row r="48" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="38"/>
-      <c r="B48" s="43" t="s">
+      <c r="A48" s="49"/>
+      <c r="B48" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="46"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A49" s="38"/>
-      <c r="B49" s="43" t="s">
+      <c r="A49" s="49"/>
+      <c r="B49" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="46"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A50" s="39"/>
-      <c r="B50" s="43" t="s">
+      <c r="A50" s="53"/>
+      <c r="B50" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="57"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:G27"/>
-    <mergeCell ref="H5:H27"/>
-    <mergeCell ref="I5:I27"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:F41"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="G28:G50"/>
     <mergeCell ref="H28:H50"/>
@@ -3455,18 +3427,37 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:G27"/>
+    <mergeCell ref="H5:H27"/>
+    <mergeCell ref="I5:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3482,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E4222C-B6F0-CA43-929A-A25489896A98}">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3499,11 +3490,11 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
@@ -3542,179 +3533,179 @@
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="75">
         <v>1</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="73" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="74">
+      <c r="A6" s="66">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="G6" s="78"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="75"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A7" s="74"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="66"/>
+      <c r="B7" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="G7" s="78"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="75"/>
+      <c r="G7" s="74"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A8" s="74"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="66"/>
+      <c r="B8" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="G8" s="78"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="75"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A9" s="74"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="G9" s="78"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="75"/>
+      <c r="G9" s="74"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A10" s="74">
+      <c r="A10" s="66">
         <v>1.2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="73"/>
-      <c r="G10" s="78"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="75"/>
+      <c r="G10" s="74"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A11" s="74"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="66"/>
+      <c r="B11" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="73"/>
-      <c r="G11" s="78"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="75"/>
+      <c r="G11" s="74"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A12" s="74"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="66"/>
+      <c r="B12" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="73"/>
-      <c r="G12" s="78"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="75"/>
+      <c r="G12" s="74"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A13" s="74">
+      <c r="A13" s="66">
         <v>1.3</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="73"/>
-      <c r="G13" s="78"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="75"/>
+      <c r="G13" s="74"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A14" s="74"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="73"/>
-      <c r="G14" s="78"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="75"/>
+      <c r="G14" s="74"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A15" s="74"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="66"/>
+      <c r="B15" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="73"/>
-      <c r="G15" s="78"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="75"/>
+      <c r="G15" s="74"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A16" s="74"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="66"/>
+      <c r="B16" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="73"/>
-      <c r="G16" s="78"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="75"/>
+      <c r="G16" s="74"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A17" s="74">
+      <c r="A17" s="66">
         <v>1.4</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="72"/>
-      <c r="D17" s="73"/>
-      <c r="G17" s="78"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="75"/>
+      <c r="G17" s="74"/>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="74"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="73"/>
-      <c r="G18" s="78"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="75"/>
+      <c r="G18" s="74"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A19" s="74"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="73"/>
-      <c r="G19" s="78"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="75"/>
+      <c r="G19" s="74"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A20" s="74">
+      <c r="A20" s="66">
         <v>1.5</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="73"/>
-      <c r="G20" s="78"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="75"/>
+      <c r="G20" s="74"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A21" s="74"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="73"/>
-      <c r="G21" s="78"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="75"/>
+      <c r="G21" s="74"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A22" s="74"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="73"/>
-      <c r="G22" s="78"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="75"/>
+      <c r="G22" s="74"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A23" s="17">
@@ -3723,134 +3714,134 @@
       <c r="B23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="73"/>
-      <c r="G23" s="78"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="75"/>
+      <c r="G23" s="74"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A24" s="74">
+      <c r="A24" s="66">
         <v>2.1</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="73"/>
-      <c r="G24" s="78"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="75"/>
+      <c r="G24" s="74"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A25" s="74"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="66"/>
+      <c r="B25" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="73"/>
-      <c r="G25" s="78"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="75"/>
+      <c r="G25" s="74"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A26" s="74"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="66"/>
+      <c r="B26" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="72"/>
-      <c r="D26" s="73"/>
-      <c r="G26" s="78"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="75"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A27" s="70">
+      <c r="A27" s="64">
         <v>2.2000000000000002</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="73"/>
-      <c r="G27" s="78"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="75"/>
+      <c r="G27" s="74"/>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="70"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="73"/>
-      <c r="G28" s="78"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="75"/>
+      <c r="G28" s="74"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A29" s="70"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="73"/>
-      <c r="G29" s="78"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="75"/>
+      <c r="G29" s="74"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A30" s="70"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="73"/>
-      <c r="G30" s="78"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="75"/>
+      <c r="G30" s="74"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A31" s="70">
+      <c r="A31" s="64">
         <v>2.2999999999999998</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="72"/>
-      <c r="D31" s="73"/>
-      <c r="G31" s="78"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="75"/>
+      <c r="G31" s="74"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A32" s="70"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="73"/>
-      <c r="G32" s="78"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="75"/>
+      <c r="G32" s="74"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A33" s="70"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="73"/>
-      <c r="G33" s="78"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="75"/>
+      <c r="G33" s="74"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A34" s="70">
+      <c r="A34" s="64">
         <v>2.4</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="73"/>
-      <c r="G34" s="78"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="75"/>
+      <c r="G34" s="74"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A35" s="70"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="73"/>
-      <c r="G35" s="78"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="75"/>
+      <c r="G35" s="74"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A36" s="70"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="72"/>
-      <c r="D36" s="73"/>
-      <c r="G36" s="78"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="75"/>
+      <c r="G36" s="74"/>
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="17">
@@ -3859,125 +3850,125 @@
       <c r="B37" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="73"/>
-      <c r="G37" s="78"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="75"/>
+      <c r="G37" s="74"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A38" s="70">
+      <c r="A38" s="64">
         <v>3.1</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="73"/>
-      <c r="G38" s="78"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="75"/>
+      <c r="G38" s="74"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A39" s="70"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="73"/>
-      <c r="G39" s="78"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="75"/>
+      <c r="G39" s="74"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A40" s="70"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
-      <c r="G40" s="78"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="75"/>
+      <c r="G40" s="74"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A41" s="70">
+      <c r="A41" s="64">
         <v>3.2</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
-      <c r="G41" s="78"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="75"/>
+      <c r="G41" s="74"/>
     </row>
     <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="70"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="72"/>
-      <c r="D42" s="73"/>
-      <c r="G42" s="78"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="75"/>
+      <c r="G42" s="74"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A43" s="70"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
-      <c r="G43" s="78"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="75"/>
+      <c r="G43" s="74"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A44" s="70">
+      <c r="A44" s="64">
         <v>3.3</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="73"/>
-      <c r="G44" s="78"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="75"/>
+      <c r="G44" s="74"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A45" s="70"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="73"/>
-      <c r="G45" s="78"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="75"/>
+      <c r="G45" s="74"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A46" s="70"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="73"/>
-      <c r="G46" s="78"/>
+      <c r="C46" s="68"/>
+      <c r="D46" s="75"/>
+      <c r="G46" s="74"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A47" s="70">
+      <c r="A47" s="64">
         <v>3.4</v>
       </c>
       <c r="B47" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="73"/>
-      <c r="G47" s="78"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="75"/>
+      <c r="G47" s="74"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A48" s="70"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="72"/>
-      <c r="D48" s="73"/>
-      <c r="G48" s="78"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="75"/>
+      <c r="G48" s="74"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A49" s="70"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="72"/>
-      <c r="D49" s="73"/>
-      <c r="G49" s="78"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="75"/>
+      <c r="G49" s="74"/>
     </row>
     <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="17">
@@ -3986,150 +3977,150 @@
       <c r="B50" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="72" t="s">
+      <c r="C50" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="D50" s="73">
+      <c r="D50" s="75">
         <v>1</v>
       </c>
       <c r="E50" s="8"/>
-      <c r="G50" s="75" t="s">
+      <c r="G50" s="69" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A51" s="70">
+      <c r="A51" s="64">
         <v>4.0999999999999996</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="73"/>
-      <c r="G51" s="75"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="75"/>
+      <c r="G51" s="69"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A52" s="70"/>
+      <c r="A52" s="64"/>
       <c r="B52" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="73"/>
-      <c r="G52" s="75"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="75"/>
+      <c r="G52" s="69"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A53" s="70"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="73"/>
-      <c r="G53" s="75"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="75"/>
+      <c r="G53" s="69"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A54" s="70"/>
+      <c r="A54" s="64"/>
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="72"/>
-      <c r="D54" s="73"/>
-      <c r="G54" s="75"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="75"/>
+      <c r="G54" s="69"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A55" s="70">
+      <c r="A55" s="64">
         <v>4.2</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="72"/>
-      <c r="D55" s="73"/>
-      <c r="G55" s="75"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="75"/>
+      <c r="G55" s="69"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A56" s="70"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="72"/>
-      <c r="D56" s="73"/>
-      <c r="G56" s="75"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="75"/>
+      <c r="G56" s="69"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A57" s="70"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="73"/>
-      <c r="G57" s="75"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="75"/>
+      <c r="G57" s="69"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A58" s="70">
+      <c r="A58" s="64">
         <v>4.3</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="72"/>
-      <c r="D58" s="73"/>
-      <c r="G58" s="75"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="75"/>
+      <c r="G58" s="69"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A59" s="70"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="72"/>
-      <c r="D59" s="73"/>
-      <c r="G59" s="75"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="75"/>
+      <c r="G59" s="69"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A60" s="70"/>
+      <c r="A60" s="64"/>
       <c r="B60" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="72"/>
-      <c r="D60" s="73"/>
-      <c r="G60" s="75"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="75"/>
+      <c r="G60" s="69"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A61" s="70">
+      <c r="A61" s="64">
         <v>4.4000000000000004</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="73"/>
-      <c r="G61" s="75"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="75"/>
+      <c r="G61" s="69"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A62" s="70"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="72"/>
-      <c r="D62" s="73"/>
-      <c r="G62" s="75"/>
+      <c r="C62" s="68"/>
+      <c r="D62" s="75"/>
+      <c r="G62" s="69"/>
     </row>
     <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="70"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="72"/>
-      <c r="D63" s="73"/>
-      <c r="G63" s="75"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="75"/>
+      <c r="G63" s="69"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A64" s="70"/>
+      <c r="A64" s="64"/>
       <c r="B64" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="73"/>
-      <c r="G64" s="75"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="75"/>
+      <c r="G64" s="69"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A65" s="17">
@@ -4138,125 +4129,125 @@
       <c r="B65" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="73"/>
-      <c r="G65" s="75"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="75"/>
+      <c r="G65" s="69"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A66" s="70">
+      <c r="A66" s="64">
         <v>5.0999999999999996</v>
       </c>
       <c r="B66" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="72"/>
-      <c r="D66" s="73"/>
-      <c r="G66" s="75"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="75"/>
+      <c r="G66" s="69"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A67" s="70"/>
+      <c r="A67" s="64"/>
       <c r="B67" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="73"/>
-      <c r="G67" s="75"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="75"/>
+      <c r="G67" s="69"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A68" s="70"/>
+      <c r="A68" s="64"/>
       <c r="B68" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="72"/>
-      <c r="D68" s="73"/>
-      <c r="G68" s="75"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="75"/>
+      <c r="G68" s="69"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A69" s="70">
+      <c r="A69" s="64">
         <v>5.2</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="72"/>
-      <c r="D69" s="73"/>
-      <c r="G69" s="75"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="75"/>
+      <c r="G69" s="69"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A70" s="70"/>
+      <c r="A70" s="64"/>
       <c r="B70" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="72"/>
-      <c r="D70" s="73"/>
-      <c r="G70" s="75"/>
+      <c r="C70" s="68"/>
+      <c r="D70" s="75"/>
+      <c r="G70" s="69"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A71" s="70"/>
+      <c r="A71" s="64"/>
       <c r="B71" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="72"/>
-      <c r="D71" s="73"/>
-      <c r="G71" s="75"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="75"/>
+      <c r="G71" s="69"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A72" s="70">
+      <c r="A72" s="64">
         <v>5.3</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="72"/>
-      <c r="D72" s="73"/>
-      <c r="G72" s="75"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="75"/>
+      <c r="G72" s="69"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A73" s="70"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="73"/>
-      <c r="G73" s="75"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="75"/>
+      <c r="G73" s="69"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A74" s="70"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="72"/>
-      <c r="D74" s="73"/>
-      <c r="G74" s="75"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="75"/>
+      <c r="G74" s="69"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A75" s="70">
+      <c r="A75" s="64">
         <v>5.4</v>
       </c>
       <c r="B75" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="72"/>
-      <c r="D75" s="73"/>
-      <c r="G75" s="75"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="75"/>
+      <c r="G75" s="69"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A76" s="70"/>
+      <c r="A76" s="64"/>
       <c r="B76" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="72"/>
-      <c r="D76" s="73"/>
-      <c r="G76" s="75"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="75"/>
+      <c r="G76" s="69"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A77" s="70"/>
+      <c r="A77" s="64"/>
       <c r="B77" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="73"/>
-      <c r="G77" s="75"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="75"/>
+      <c r="G77" s="69"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A78" s="17">
@@ -4265,199 +4256,199 @@
       <c r="B78" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="72"/>
-      <c r="D78" s="73"/>
-      <c r="G78" s="75"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="75"/>
+      <c r="G78" s="69"/>
     </row>
     <row r="79" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A79" s="74">
+      <c r="A79" s="66">
         <v>6.1</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="72"/>
-      <c r="D79" s="73"/>
-      <c r="G79" s="75"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="75"/>
+      <c r="G79" s="69"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A80" s="74"/>
+      <c r="A80" s="66"/>
       <c r="B80" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="72"/>
-      <c r="D80" s="73"/>
-      <c r="G80" s="75"/>
+      <c r="C80" s="68"/>
+      <c r="D80" s="75"/>
+      <c r="G80" s="69"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A81" s="74"/>
+      <c r="A81" s="66"/>
       <c r="B81" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="72"/>
-      <c r="D81" s="73"/>
-      <c r="G81" s="75"/>
+      <c r="C81" s="68"/>
+      <c r="D81" s="75"/>
+      <c r="G81" s="69"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A82" s="74"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="72"/>
-      <c r="D82" s="73"/>
-      <c r="G82" s="75"/>
+      <c r="C82" s="68"/>
+      <c r="D82" s="75"/>
+      <c r="G82" s="69"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A83" s="74"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="72"/>
-      <c r="D83" s="73"/>
-      <c r="G83" s="75"/>
+      <c r="C83" s="68"/>
+      <c r="D83" s="75"/>
+      <c r="G83" s="69"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A84" s="70">
+      <c r="A84" s="64">
         <v>6.2</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="72"/>
-      <c r="D84" s="73"/>
-      <c r="G84" s="75"/>
+      <c r="C84" s="68"/>
+      <c r="D84" s="75"/>
+      <c r="G84" s="69"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A85" s="70"/>
+      <c r="A85" s="64"/>
       <c r="B85" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="72"/>
-      <c r="D85" s="73"/>
-      <c r="G85" s="75"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="75"/>
+      <c r="G85" s="69"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A86" s="70"/>
+      <c r="A86" s="64"/>
       <c r="B86" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="72"/>
-      <c r="D86" s="73"/>
-      <c r="G86" s="75"/>
+      <c r="C86" s="68"/>
+      <c r="D86" s="75"/>
+      <c r="G86" s="69"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A87" s="70"/>
+      <c r="A87" s="64"/>
       <c r="B87" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="72"/>
-      <c r="D87" s="73"/>
-      <c r="G87" s="75"/>
+      <c r="C87" s="68"/>
+      <c r="D87" s="75"/>
+      <c r="G87" s="69"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A88" s="70"/>
+      <c r="A88" s="64"/>
       <c r="B88" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="72"/>
-      <c r="D88" s="73"/>
-      <c r="G88" s="75"/>
+      <c r="C88" s="68"/>
+      <c r="D88" s="75"/>
+      <c r="G88" s="69"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A89" s="70">
+      <c r="A89" s="64">
         <v>6.3</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="72"/>
-      <c r="D89" s="73"/>
-      <c r="G89" s="75"/>
+      <c r="C89" s="68"/>
+      <c r="D89" s="75"/>
+      <c r="G89" s="69"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A90" s="70"/>
+      <c r="A90" s="64"/>
       <c r="B90" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="72"/>
-      <c r="D90" s="73"/>
-      <c r="G90" s="75"/>
+      <c r="C90" s="68"/>
+      <c r="D90" s="75"/>
+      <c r="G90" s="69"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A91" s="70"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="72"/>
-      <c r="D91" s="73"/>
-      <c r="G91" s="75"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="75"/>
+      <c r="G91" s="69"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A92" s="70">
+      <c r="A92" s="64">
         <v>6.4</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="72"/>
-      <c r="D92" s="73"/>
-      <c r="G92" s="75"/>
+      <c r="C92" s="68"/>
+      <c r="D92" s="75"/>
+      <c r="G92" s="69"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A93" s="70"/>
+      <c r="A93" s="64"/>
       <c r="B93" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="72"/>
-      <c r="D93" s="73"/>
-      <c r="G93" s="75"/>
+      <c r="C93" s="68"/>
+      <c r="D93" s="75"/>
+      <c r="G93" s="69"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A94" s="70"/>
+      <c r="A94" s="64"/>
       <c r="B94" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="72"/>
-      <c r="D94" s="73"/>
-      <c r="G94" s="75"/>
+      <c r="C94" s="68"/>
+      <c r="D94" s="75"/>
+      <c r="G94" s="69"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A95" s="70">
+      <c r="A95" s="64">
         <v>6.5</v>
       </c>
       <c r="B95" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C95" s="72"/>
-      <c r="D95" s="73"/>
-      <c r="G95" s="75"/>
+      <c r="C95" s="68"/>
+      <c r="D95" s="75"/>
+      <c r="G95" s="69"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A96" s="70"/>
+      <c r="A96" s="64"/>
       <c r="B96" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="72"/>
-      <c r="D96" s="73"/>
-      <c r="G96" s="75"/>
+      <c r="C96" s="68"/>
+      <c r="D96" s="75"/>
+      <c r="G96" s="69"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A97" s="70"/>
+      <c r="A97" s="64"/>
       <c r="B97" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C97" s="72"/>
-      <c r="D97" s="73"/>
-      <c r="G97" s="75"/>
+      <c r="C97" s="68"/>
+      <c r="D97" s="75"/>
+      <c r="G97" s="69"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A98" s="70"/>
+      <c r="A98" s="64"/>
       <c r="B98" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C98" s="72"/>
-      <c r="D98" s="73"/>
-      <c r="G98" s="75"/>
+      <c r="C98" s="68"/>
+      <c r="D98" s="75"/>
+      <c r="G98" s="69"/>
     </row>
     <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A99" s="17">
@@ -4466,132 +4457,132 @@
       <c r="B99" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="76" t="s">
+      <c r="C99" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="D99" s="80">
+      <c r="D99" s="65">
         <v>1</v>
       </c>
       <c r="E99" s="8"/>
-      <c r="G99" s="79" t="s">
+      <c r="G99" s="67" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A100" s="70">
+      <c r="A100" s="64">
         <v>7.1</v>
       </c>
       <c r="B100" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="76"/>
-      <c r="D100" s="80"/>
-      <c r="G100" s="79"/>
+      <c r="C100" s="71"/>
+      <c r="D100" s="65"/>
+      <c r="G100" s="67"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A101" s="70"/>
+      <c r="A101" s="64"/>
       <c r="B101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="76"/>
-      <c r="D101" s="80"/>
-      <c r="G101" s="79"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="65"/>
+      <c r="G101" s="67"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A102" s="70"/>
+      <c r="A102" s="64"/>
       <c r="B102" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="76"/>
-      <c r="D102" s="80"/>
-      <c r="G102" s="79"/>
+      <c r="C102" s="71"/>
+      <c r="D102" s="65"/>
+      <c r="G102" s="67"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A103" s="70">
+      <c r="A103" s="64">
         <v>7.2</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="76"/>
-      <c r="D103" s="80"/>
-      <c r="G103" s="79"/>
+      <c r="C103" s="71"/>
+      <c r="D103" s="65"/>
+      <c r="G103" s="67"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A104" s="70"/>
+      <c r="A104" s="64"/>
       <c r="B104" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="76"/>
-      <c r="D104" s="80"/>
-      <c r="G104" s="79"/>
+      <c r="C104" s="71"/>
+      <c r="D104" s="65"/>
+      <c r="G104" s="67"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A105" s="70"/>
+      <c r="A105" s="64"/>
       <c r="B105" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="76"/>
-      <c r="D105" s="80"/>
-      <c r="G105" s="79"/>
+      <c r="C105" s="71"/>
+      <c r="D105" s="65"/>
+      <c r="G105" s="67"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A106" s="70">
+      <c r="A106" s="64">
         <v>7.3</v>
       </c>
       <c r="B106" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="76"/>
-      <c r="D106" s="80"/>
-      <c r="G106" s="79"/>
+      <c r="C106" s="71"/>
+      <c r="D106" s="65"/>
+      <c r="G106" s="67"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A107" s="70"/>
+      <c r="A107" s="64"/>
       <c r="B107" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="76"/>
-      <c r="D107" s="80"/>
-      <c r="G107" s="79"/>
+      <c r="C107" s="71"/>
+      <c r="D107" s="65"/>
+      <c r="G107" s="67"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A108" s="70"/>
+      <c r="A108" s="64"/>
       <c r="B108" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="76"/>
-      <c r="D108" s="80"/>
-      <c r="G108" s="79"/>
+      <c r="C108" s="71"/>
+      <c r="D108" s="65"/>
+      <c r="G108" s="67"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A109" s="70">
+      <c r="A109" s="64">
         <v>7.4</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="76"/>
-      <c r="D109" s="80"/>
-      <c r="G109" s="79"/>
+      <c r="C109" s="71"/>
+      <c r="D109" s="65"/>
+      <c r="G109" s="67"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A110" s="70"/>
+      <c r="A110" s="64"/>
       <c r="B110" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="76"/>
-      <c r="D110" s="80"/>
-      <c r="G110" s="79"/>
+      <c r="C110" s="71"/>
+      <c r="D110" s="65"/>
+      <c r="G110" s="67"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A111" s="70"/>
+      <c r="A111" s="64"/>
       <c r="B111" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C111" s="76"/>
-      <c r="D111" s="80"/>
-      <c r="G111" s="79"/>
+      <c r="C111" s="71"/>
+      <c r="D111" s="65"/>
+      <c r="G111" s="67"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A112" s="21">
@@ -4600,9 +4591,9 @@
       <c r="B112" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C112" s="76"/>
-      <c r="D112" s="80"/>
-      <c r="G112" s="79"/>
+      <c r="C112" s="71"/>
+      <c r="D112" s="65"/>
+      <c r="G112" s="67"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A113" s="21">
@@ -4611,101 +4602,101 @@
       <c r="B113" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="76"/>
-      <c r="D113" s="80"/>
-      <c r="G113" s="79"/>
+      <c r="C113" s="71"/>
+      <c r="D113" s="65"/>
+      <c r="G113" s="67"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A114" s="70">
+      <c r="A114" s="64">
         <v>8.1</v>
       </c>
       <c r="B114" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C114" s="76"/>
-      <c r="D114" s="80"/>
-      <c r="G114" s="79"/>
+      <c r="C114" s="71"/>
+      <c r="D114" s="65"/>
+      <c r="G114" s="67"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A115" s="70"/>
+      <c r="A115" s="64"/>
       <c r="B115" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C115" s="76"/>
-      <c r="D115" s="80"/>
-      <c r="G115" s="79"/>
+      <c r="C115" s="71"/>
+      <c r="D115" s="65"/>
+      <c r="G115" s="67"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A116" s="70"/>
+      <c r="A116" s="64"/>
       <c r="B116" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="C116" s="76"/>
-      <c r="D116" s="80"/>
-      <c r="G116" s="79"/>
+      <c r="C116" s="71"/>
+      <c r="D116" s="65"/>
+      <c r="G116" s="67"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A117" s="70"/>
+      <c r="A117" s="64"/>
       <c r="B117" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="C117" s="76"/>
-      <c r="D117" s="80"/>
-      <c r="G117" s="79"/>
+      <c r="C117" s="71"/>
+      <c r="D117" s="65"/>
+      <c r="G117" s="67"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A118" s="70"/>
+      <c r="A118" s="64"/>
       <c r="B118" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="C118" s="76"/>
-      <c r="D118" s="80"/>
-      <c r="G118" s="79"/>
+      <c r="C118" s="71"/>
+      <c r="D118" s="65"/>
+      <c r="G118" s="67"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A119" s="70"/>
+      <c r="A119" s="64"/>
       <c r="B119" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="C119" s="76"/>
-      <c r="D119" s="80"/>
-      <c r="G119" s="79"/>
+      <c r="C119" s="71"/>
+      <c r="D119" s="65"/>
+      <c r="G119" s="67"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A120" s="70"/>
+      <c r="A120" s="64"/>
       <c r="B120" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="C120" s="76"/>
-      <c r="D120" s="80"/>
-      <c r="G120" s="79"/>
+      <c r="C120" s="71"/>
+      <c r="D120" s="65"/>
+      <c r="G120" s="67"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A121" s="70"/>
+      <c r="A121" s="64"/>
       <c r="B121" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C121" s="76"/>
-      <c r="D121" s="80"/>
-      <c r="G121" s="79"/>
+      <c r="C121" s="71"/>
+      <c r="D121" s="65"/>
+      <c r="G121" s="67"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A122" s="70"/>
+      <c r="A122" s="64"/>
       <c r="B122" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C122" s="76"/>
-      <c r="D122" s="80"/>
-      <c r="G122" s="79"/>
+      <c r="C122" s="71"/>
+      <c r="D122" s="65"/>
+      <c r="G122" s="67"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A123" s="70"/>
+      <c r="A123" s="64"/>
       <c r="B123" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="C123" s="76"/>
-      <c r="D123" s="80"/>
-      <c r="G123" s="79"/>
+      <c r="C123" s="71"/>
+      <c r="D123" s="65"/>
+      <c r="G123" s="67"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A124" s="17">
@@ -4714,175 +4705,175 @@
       <c r="B124" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C124" s="76" t="s">
+      <c r="C124" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="D124" s="80">
+      <c r="D124" s="65">
         <v>0.75</v>
       </c>
       <c r="E124" s="8"/>
-      <c r="G124" s="79"/>
+      <c r="G124" s="67"/>
     </row>
     <row r="125" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A125" s="74">
+      <c r="A125" s="66">
         <v>9.1</v>
       </c>
       <c r="B125" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C125" s="76"/>
-      <c r="D125" s="80"/>
-      <c r="G125" s="79"/>
+      <c r="C125" s="71"/>
+      <c r="D125" s="65"/>
+      <c r="G125" s="67"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A126" s="74"/>
+      <c r="A126" s="66"/>
       <c r="B126" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C126" s="76"/>
-      <c r="D126" s="80"/>
-      <c r="G126" s="79"/>
+      <c r="C126" s="71"/>
+      <c r="D126" s="65"/>
+      <c r="G126" s="67"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A127" s="74"/>
+      <c r="A127" s="66"/>
       <c r="B127" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C127" s="76"/>
-      <c r="D127" s="80"/>
-      <c r="G127" s="79"/>
+      <c r="C127" s="71"/>
+      <c r="D127" s="65"/>
+      <c r="G127" s="67"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A128" s="74"/>
+      <c r="A128" s="66"/>
       <c r="B128" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C128" s="76"/>
-      <c r="D128" s="80"/>
-      <c r="G128" s="79"/>
+      <c r="C128" s="71"/>
+      <c r="D128" s="65"/>
+      <c r="G128" s="67"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A129" s="74"/>
+      <c r="A129" s="66"/>
       <c r="B129" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C129" s="76"/>
-      <c r="D129" s="80"/>
-      <c r="G129" s="79"/>
+      <c r="C129" s="71"/>
+      <c r="D129" s="65"/>
+      <c r="G129" s="67"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A130" s="70">
+      <c r="A130" s="64">
         <v>9.1999999999999993</v>
       </c>
       <c r="B130" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C130" s="76"/>
-      <c r="D130" s="80"/>
-      <c r="G130" s="79"/>
+      <c r="C130" s="71"/>
+      <c r="D130" s="65"/>
+      <c r="G130" s="67"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A131" s="70"/>
+      <c r="A131" s="64"/>
       <c r="B131" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C131" s="76"/>
-      <c r="D131" s="80"/>
-      <c r="G131" s="79"/>
+      <c r="C131" s="71"/>
+      <c r="D131" s="65"/>
+      <c r="G131" s="67"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A132" s="70"/>
+      <c r="A132" s="64"/>
       <c r="B132" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C132" s="76"/>
-      <c r="D132" s="80"/>
-      <c r="G132" s="79"/>
+      <c r="C132" s="71"/>
+      <c r="D132" s="65"/>
+      <c r="G132" s="67"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A133" s="70"/>
+      <c r="A133" s="64"/>
       <c r="B133" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C133" s="76"/>
-      <c r="D133" s="80"/>
-      <c r="G133" s="79"/>
+      <c r="C133" s="71"/>
+      <c r="D133" s="65"/>
+      <c r="G133" s="67"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A134" s="70">
+      <c r="A134" s="64">
         <v>9.3000000000000007</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C134" s="76"/>
-      <c r="D134" s="80"/>
-      <c r="G134" s="79"/>
+      <c r="C134" s="71"/>
+      <c r="D134" s="65"/>
+      <c r="G134" s="67"/>
     </row>
     <row r="135" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A135" s="70"/>
+      <c r="A135" s="64"/>
       <c r="B135" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C135" s="76"/>
-      <c r="D135" s="80"/>
-      <c r="G135" s="79"/>
+      <c r="C135" s="71"/>
+      <c r="D135" s="65"/>
+      <c r="G135" s="67"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A136" s="70"/>
+      <c r="A136" s="64"/>
       <c r="B136" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C136" s="76"/>
-      <c r="D136" s="80"/>
-      <c r="G136" s="79"/>
+      <c r="C136" s="71"/>
+      <c r="D136" s="65"/>
+      <c r="G136" s="67"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A137" s="70"/>
+      <c r="A137" s="64"/>
       <c r="B137" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C137" s="76"/>
-      <c r="D137" s="80"/>
-      <c r="G137" s="79"/>
+      <c r="C137" s="71"/>
+      <c r="D137" s="65"/>
+      <c r="G137" s="67"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A138" s="70">
+      <c r="A138" s="64">
         <v>9.4</v>
       </c>
       <c r="B138" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C138" s="76"/>
-      <c r="D138" s="80"/>
-      <c r="G138" s="79"/>
+      <c r="C138" s="71"/>
+      <c r="D138" s="65"/>
+      <c r="G138" s="67"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A139" s="70"/>
+      <c r="A139" s="64"/>
       <c r="B139" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C139" s="76"/>
-      <c r="D139" s="80"/>
-      <c r="G139" s="79"/>
+      <c r="C139" s="71"/>
+      <c r="D139" s="65"/>
+      <c r="G139" s="67"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A140" s="70"/>
+      <c r="A140" s="64"/>
       <c r="B140" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="76"/>
-      <c r="D140" s="80"/>
-      <c r="G140" s="79"/>
+      <c r="C140" s="71"/>
+      <c r="D140" s="65"/>
+      <c r="G140" s="67"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A141" s="70"/>
+      <c r="A141" s="64"/>
       <c r="B141" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C141" s="76"/>
-      <c r="D141" s="80"/>
-      <c r="G141" s="79"/>
+      <c r="C141" s="71"/>
+      <c r="D141" s="65"/>
+      <c r="G141" s="67"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A142" s="17">
@@ -4891,14 +4882,14 @@
       <c r="B142" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="72" t="s">
+      <c r="C142" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="D142" s="80">
+      <c r="D142" s="65">
         <v>1.75</v>
       </c>
       <c r="E142" s="8"/>
-      <c r="G142" s="79"/>
+      <c r="G142" s="67"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A143" s="21">
@@ -4907,9 +4898,9 @@
       <c r="B143" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="72"/>
-      <c r="D143" s="80"/>
-      <c r="G143" s="79"/>
+      <c r="C143" s="68"/>
+      <c r="D143" s="65"/>
+      <c r="G143" s="67"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A144" s="17">
@@ -4918,196 +4909,206 @@
       <c r="B144" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C144" s="76" t="s">
+      <c r="C144" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="D144" s="80">
+      <c r="D144" s="65">
         <v>0.5</v>
       </c>
       <c r="E144" s="8"/>
-      <c r="G144" s="75"/>
+      <c r="G144" s="69"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A145" s="70">
+      <c r="A145" s="64">
         <v>11.1</v>
       </c>
       <c r="B145" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C145" s="82"/>
-      <c r="D145" s="80"/>
-      <c r="G145" s="75"/>
+      <c r="C145" s="72"/>
+      <c r="D145" s="65"/>
+      <c r="G145" s="69"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A146" s="70"/>
+      <c r="A146" s="64"/>
       <c r="B146" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C146" s="82"/>
-      <c r="D146" s="80"/>
-      <c r="G146" s="75"/>
+      <c r="C146" s="72"/>
+      <c r="D146" s="65"/>
+      <c r="G146" s="69"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A147" s="70"/>
+      <c r="A147" s="64"/>
       <c r="B147" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C147" s="82"/>
-      <c r="D147" s="80"/>
-      <c r="G147" s="75"/>
+      <c r="C147" s="72"/>
+      <c r="D147" s="65"/>
+      <c r="G147" s="69"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A148" s="70">
+      <c r="A148" s="64">
         <v>11.2</v>
       </c>
       <c r="B148" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C148" s="82"/>
-      <c r="D148" s="80"/>
-      <c r="G148" s="75"/>
+      <c r="C148" s="72"/>
+      <c r="D148" s="65"/>
+      <c r="G148" s="69"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A149" s="70"/>
+      <c r="A149" s="64"/>
       <c r="B149" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C149" s="82"/>
-      <c r="D149" s="80"/>
-      <c r="G149" s="75"/>
+      <c r="C149" s="72"/>
+      <c r="D149" s="65"/>
+      <c r="G149" s="69"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A150" s="70"/>
+      <c r="A150" s="64"/>
       <c r="B150" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C150" s="82"/>
-      <c r="D150" s="80"/>
-      <c r="G150" s="75"/>
+      <c r="C150" s="72"/>
+      <c r="D150" s="65"/>
+      <c r="G150" s="69"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A151" s="81">
+      <c r="A151" s="70">
         <v>11.3</v>
       </c>
       <c r="B151" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C151" s="82"/>
-      <c r="D151" s="80"/>
-      <c r="G151" s="75"/>
+      <c r="C151" s="72"/>
+      <c r="D151" s="65"/>
+      <c r="G151" s="69"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A152" s="81"/>
+      <c r="A152" s="70"/>
       <c r="B152" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="82"/>
-      <c r="D152" s="80"/>
-      <c r="G152" s="75"/>
+      <c r="C152" s="72"/>
+      <c r="D152" s="65"/>
+      <c r="G152" s="69"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A153" s="81"/>
+      <c r="A153" s="70"/>
       <c r="B153" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C153" s="82"/>
-      <c r="D153" s="80"/>
-      <c r="G153" s="75"/>
+      <c r="C153" s="72"/>
+      <c r="D153" s="65"/>
+      <c r="G153" s="69"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A154" s="81"/>
+      <c r="A154" s="70"/>
       <c r="B154" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C154" s="82"/>
-      <c r="D154" s="80"/>
-      <c r="G154" s="75"/>
+      <c r="C154" s="72"/>
+      <c r="D154" s="65"/>
+      <c r="G154" s="69"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A155" s="81">
+      <c r="A155" s="70">
         <v>11.4</v>
       </c>
       <c r="B155" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C155" s="82"/>
-      <c r="D155" s="80"/>
-      <c r="G155" s="75"/>
+      <c r="C155" s="72"/>
+      <c r="D155" s="65"/>
+      <c r="G155" s="69"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A156" s="81"/>
+      <c r="A156" s="70"/>
       <c r="B156" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C156" s="82"/>
-      <c r="D156" s="80"/>
-      <c r="G156" s="75"/>
+      <c r="C156" s="72"/>
+      <c r="D156" s="65"/>
+      <c r="G156" s="69"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A157" s="81"/>
+      <c r="A157" s="70"/>
       <c r="B157" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C157" s="82"/>
-      <c r="D157" s="80"/>
-      <c r="G157" s="75"/>
+      <c r="C157" s="72"/>
+      <c r="D157" s="65"/>
+      <c r="G157" s="69"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A158" s="81">
+      <c r="A158" s="70">
         <v>11.5</v>
       </c>
       <c r="B158" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C158" s="82"/>
-      <c r="D158" s="80"/>
-      <c r="G158" s="75"/>
+      <c r="C158" s="72"/>
+      <c r="D158" s="65"/>
+      <c r="G158" s="69"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A159" s="81"/>
+      <c r="A159" s="70"/>
       <c r="B159" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C159" s="82"/>
-      <c r="D159" s="80"/>
-      <c r="G159" s="75"/>
+      <c r="C159" s="72"/>
+      <c r="D159" s="65"/>
+      <c r="G159" s="69"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A160" s="81"/>
+      <c r="A160" s="70"/>
       <c r="B160" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C160" s="82"/>
-      <c r="D160" s="80"/>
-      <c r="G160" s="75"/>
+      <c r="C160" s="72"/>
+      <c r="D160" s="65"/>
+      <c r="G160" s="69"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A161" s="81"/>
+      <c r="A161" s="70"/>
       <c r="B161" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C161" s="82"/>
-      <c r="D161" s="80"/>
-      <c r="G161" s="75"/>
+      <c r="C161" s="72"/>
+      <c r="D161" s="65"/>
+      <c r="G161" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="D124:D141"/>
-    <mergeCell ref="A125:A129"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="G144:G161"/>
-    <mergeCell ref="D144:D161"/>
-    <mergeCell ref="A148:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C5:C49"/>
+    <mergeCell ref="D5:D49"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C50:C98"/>
+    <mergeCell ref="D50:D98"/>
+    <mergeCell ref="G50:G98"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A95:A98"/>
     <mergeCell ref="C99:C123"/>
     <mergeCell ref="G5:G49"/>
     <mergeCell ref="G99:G141"/>
@@ -5124,32 +5125,22 @@
     <mergeCell ref="A89:A91"/>
     <mergeCell ref="A92:A94"/>
     <mergeCell ref="D99:D123"/>
-    <mergeCell ref="C50:C98"/>
-    <mergeCell ref="D50:D98"/>
-    <mergeCell ref="G50:G98"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="C5:C49"/>
-    <mergeCell ref="D5:D49"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="G144:G161"/>
+    <mergeCell ref="D144:D161"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="D124:D141"/>
+    <mergeCell ref="A125:A129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C# Day4 Abstract Class/Interface Topics
</commit_message>
<xml_diff>
--- a/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
+++ b/CP_Platform_Solution_.Net_v1.4-Phase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anami\WiproBatch-25April\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9071FB-BCE4-4412-9E5F-171635E17D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB23270-8013-4E76-A0DA-053C8B47A7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" activeTab="2" xr2:uid="{A334C00E-DF14-8E42-AC33-43AB2B07B0C8}"/>
   </bookViews>
@@ -2004,7 +2004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2114,21 +2114,87 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2138,110 +2204,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2659,16 +2662,16 @@
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="9" t="s">
@@ -2687,13 +2690,13 @@
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
@@ -2708,187 +2711,187 @@
       <c r="A5" s="15">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="57">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A6" s="50">
+      <c r="A6" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="58"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A7" s="51"/>
-      <c r="B7" s="57" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A8" s="51"/>
-      <c r="B8" s="57" t="s">
+      <c r="A8" s="43"/>
+      <c r="B8" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="58"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A9" s="51"/>
-      <c r="B9" s="57" t="s">
+      <c r="A9" s="43"/>
+      <c r="B9" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A10" s="51"/>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A11" s="51"/>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="43"/>
+      <c r="B11" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="48"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A12" s="55"/>
-      <c r="B12" s="60" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="48"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A13" s="50">
+      <c r="A13" s="42">
         <v>1.2</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A14" s="51"/>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A15" s="51"/>
-      <c r="B15" s="57" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A16" s="55"/>
-      <c r="B16" s="57" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A17" s="50">
+      <c r="A17" s="42">
         <v>1.3</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A18" s="51"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="30" t="s">
         <v>186</v>
       </c>
@@ -2896,12 +2899,12 @@
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="48"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A19" s="51"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="26" t="s">
         <v>187</v>
       </c>
@@ -2909,318 +2912,318 @@
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="48"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="58"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A20" s="50">
+      <c r="A20" s="42">
         <v>1.4</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="48"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="58"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A21" s="51"/>
-      <c r="B21" s="57" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="58"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A22" s="51"/>
-      <c r="B22" s="57" t="s">
+      <c r="A22" s="43"/>
+      <c r="B22" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="55"/>
-      <c r="B23" s="57" t="s">
+      <c r="A23" s="44"/>
+      <c r="B23" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A24" s="50">
+      <c r="A24" s="42">
         <v>1.5</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="48"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A25" s="51"/>
-      <c r="B25" s="57" t="s">
+      <c r="A25" s="43"/>
+      <c r="B25" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A26" s="51"/>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="43"/>
+      <c r="B26" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A27" s="55"/>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="44"/>
+      <c r="B27" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" s="15">
         <v>2</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="63" t="s">
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="63" t="s">
+      <c r="H28" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="I28" s="47">
+      <c r="I28" s="57">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A29" s="50">
+      <c r="A29" s="42">
         <v>2.1</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="48"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A30" s="51"/>
-      <c r="B30" s="57" t="s">
+      <c r="A30" s="43"/>
+      <c r="B30" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="58"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A31" s="51"/>
-      <c r="B31" s="57" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="58"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A32" s="55"/>
-      <c r="B32" s="57" t="s">
+      <c r="A32" s="44"/>
+      <c r="B32" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A33" s="50">
+      <c r="A33" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="48"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="58"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A34" s="51"/>
-      <c r="B34" s="57" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="58"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A35" s="51"/>
-      <c r="B35" s="57" t="s">
+      <c r="A35" s="43"/>
+      <c r="B35" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="58"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A36" s="55"/>
-      <c r="B36" s="57" t="s">
+      <c r="A36" s="44"/>
+      <c r="B36" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="58"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A37" s="50">
+      <c r="A37" s="42">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="45" t="s">
         <v>207</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="48"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A38" s="51"/>
-      <c r="B38" s="57" t="s">
+      <c r="A38" s="43"/>
+      <c r="B38" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="58"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A39" s="51"/>
-      <c r="B39" s="57" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="58"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A40" s="55"/>
-      <c r="B40" s="57" t="s">
+      <c r="A40" s="44"/>
+      <c r="B40" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="48"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="58"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A41" s="50">
+      <c r="A41" s="42">
         <v>2.4</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="48"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="58"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A42" s="51"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="30" t="s">
         <v>212</v>
       </c>
@@ -3228,12 +3231,12 @@
       <c r="D42" s="31"/>
       <c r="E42" s="31"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="48"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A43" s="55"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="30" t="s">
         <v>213</v>
       </c>
@@ -3241,27 +3244,27 @@
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="48"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="58"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A44" s="50">
+      <c r="A44" s="42">
         <v>2.5</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="48"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="58"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A45" s="51"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="30" t="s">
         <v>215</v>
       </c>
@@ -3269,12 +3272,12 @@
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="48"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="58"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A46" s="55"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="30" t="s">
         <v>216</v>
       </c>
@@ -3282,78 +3285,97 @@
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="48"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="58"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A47" s="50">
+      <c r="A47" s="42">
         <v>2.6</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="48"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="58"/>
     </row>
     <row r="48" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="51"/>
-      <c r="B48" s="57" t="s">
+      <c r="A48" s="43"/>
+      <c r="B48" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="48"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="58"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A49" s="51"/>
-      <c r="B49" s="57" t="s">
+      <c r="A49" s="43"/>
+      <c r="B49" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="58"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A50" s="55"/>
-      <c r="B50" s="57" t="s">
+      <c r="A50" s="44"/>
+      <c r="B50" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:G27"/>
+    <mergeCell ref="H5:H27"/>
+    <mergeCell ref="I5:I27"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="G28:G50"/>
     <mergeCell ref="H28:H50"/>
@@ -3370,37 +3392,18 @@
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:F37"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="G5:G27"/>
-    <mergeCell ref="H5:H27"/>
-    <mergeCell ref="I5:I27"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3416,8 +3419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E4222C-B6F0-CA43-929A-A25489896A98}">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G49"/>
+    <sheetView tabSelected="1" topLeftCell="D99" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99:G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -3433,11 +3436,11 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
@@ -3476,179 +3479,179 @@
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="77">
+      <c r="D5" s="72">
         <v>1</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="76" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="68">
+      <c r="A6" s="73">
         <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="77"/>
-      <c r="G6" s="76"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="G6" s="77"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A7" s="68"/>
+      <c r="A7" s="73"/>
       <c r="B7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="77"/>
-      <c r="G7" s="76"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="G7" s="77"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A8" s="68"/>
+      <c r="A8" s="73"/>
       <c r="B8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="77"/>
-      <c r="G8" s="76"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="G8" s="77"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A9" s="68"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="77"/>
-      <c r="G9" s="76"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="G9" s="77"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A10" s="68">
+      <c r="A10" s="73">
         <v>1.2</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="77"/>
-      <c r="G10" s="76"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="G10" s="77"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A11" s="68"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="77"/>
-      <c r="G11" s="76"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="G11" s="77"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A12" s="68"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="77"/>
-      <c r="G12" s="76"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="72"/>
+      <c r="G12" s="77"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A13" s="68">
+      <c r="A13" s="73">
         <v>1.3</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="77"/>
-      <c r="G13" s="76"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="G13" s="77"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A14" s="68"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="77"/>
-      <c r="G14" s="76"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="72"/>
+      <c r="G14" s="77"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A15" s="68"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="77"/>
-      <c r="G15" s="76"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72"/>
+      <c r="G15" s="77"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A16" s="68"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="77"/>
-      <c r="G16" s="76"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="G16" s="77"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A17" s="68">
+      <c r="A17" s="73">
         <v>1.4</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="77"/>
-      <c r="G17" s="76"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
+      <c r="G17" s="77"/>
     </row>
     <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="68"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="77"/>
-      <c r="G18" s="76"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="72"/>
+      <c r="G18" s="77"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A19" s="68"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="77"/>
-      <c r="G19" s="76"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="72"/>
+      <c r="G19" s="77"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A20" s="68">
+      <c r="A20" s="73">
         <v>1.5</v>
       </c>
       <c r="B20" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="77"/>
-      <c r="G20" s="76"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="72"/>
+      <c r="G20" s="77"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A21" s="68"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="77"/>
-      <c r="G21" s="76"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="72"/>
+      <c r="G21" s="77"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A22" s="68"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="77"/>
-      <c r="G22" s="76"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="72"/>
+      <c r="G22" s="77"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A23" s="17">
@@ -3657,134 +3660,134 @@
       <c r="B23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="77"/>
-      <c r="G23" s="76"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="72"/>
+      <c r="G23" s="77"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A24" s="68">
+      <c r="A24" s="73">
         <v>2.1</v>
       </c>
       <c r="B24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="77"/>
-      <c r="G24" s="76"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="72"/>
+      <c r="G24" s="77"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A25" s="68"/>
+      <c r="A25" s="73"/>
       <c r="B25" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="77"/>
-      <c r="G25" s="76"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
+      <c r="G25" s="77"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A26" s="68"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="77"/>
-      <c r="G26" s="76"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="72"/>
+      <c r="G26" s="77"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A27" s="66">
+      <c r="A27" s="69">
         <v>2.2000000000000002</v>
       </c>
       <c r="B27" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="77"/>
-      <c r="G27" s="76"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="72"/>
+      <c r="G27" s="77"/>
     </row>
     <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="66"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="77"/>
-      <c r="G28" s="76"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
+      <c r="G28" s="77"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A29" s="66"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="77"/>
-      <c r="G29" s="76"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="72"/>
+      <c r="G29" s="77"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A30" s="66"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="77"/>
-      <c r="G30" s="76"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="G30" s="77"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A31" s="66">
+      <c r="A31" s="69">
         <v>2.2999999999999998</v>
       </c>
       <c r="B31" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="77"/>
-      <c r="G31" s="76"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
+      <c r="G31" s="77"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A32" s="66"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="70"/>
-      <c r="D32" s="77"/>
-      <c r="G32" s="76"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="G32" s="77"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A33" s="66"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="77"/>
-      <c r="G33" s="76"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="72"/>
+      <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A34" s="66">
+      <c r="A34" s="69">
         <v>2.4</v>
       </c>
       <c r="B34" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="77"/>
-      <c r="G34" s="76"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="72"/>
+      <c r="G34" s="77"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A35" s="66"/>
+      <c r="A35" s="69"/>
       <c r="B35" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="77"/>
-      <c r="G35" s="76"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="G35" s="77"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A36" s="66"/>
+      <c r="A36" s="69"/>
       <c r="B36" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="77"/>
-      <c r="G36" s="76"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="G36" s="77"/>
     </row>
     <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="17">
@@ -3793,125 +3796,125 @@
       <c r="B37" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="77"/>
-      <c r="G37" s="76"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="G37" s="77"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A38" s="66">
+      <c r="A38" s="69">
         <v>3.1</v>
       </c>
       <c r="B38" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="70"/>
-      <c r="D38" s="77"/>
-      <c r="G38" s="76"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="72"/>
+      <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A39" s="66"/>
+      <c r="A39" s="69"/>
       <c r="B39" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="77"/>
-      <c r="G39" s="76"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="72"/>
+      <c r="G39" s="77"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A40" s="66"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="77"/>
-      <c r="G40" s="76"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="72"/>
+      <c r="G40" s="77"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A41" s="66">
+      <c r="A41" s="69">
         <v>3.2</v>
       </c>
       <c r="B41" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="77"/>
-      <c r="G41" s="76"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="72"/>
+      <c r="G41" s="77"/>
     </row>
     <row r="42" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A42" s="66"/>
+      <c r="A42" s="69"/>
       <c r="B42" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="77"/>
-      <c r="G42" s="76"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="72"/>
+      <c r="G42" s="77"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A43" s="66"/>
+      <c r="A43" s="69"/>
       <c r="B43" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="77"/>
-      <c r="G43" s="76"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="72"/>
+      <c r="G43" s="77"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A44" s="66">
+      <c r="A44" s="69">
         <v>3.3</v>
       </c>
       <c r="B44" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="77"/>
-      <c r="G44" s="76"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="72"/>
+      <c r="G44" s="77"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A45" s="66"/>
+      <c r="A45" s="69"/>
       <c r="B45" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="77"/>
-      <c r="G45" s="76"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="72"/>
+      <c r="G45" s="77"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A46" s="66"/>
+      <c r="A46" s="69"/>
       <c r="B46" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="70"/>
-      <c r="D46" s="77"/>
-      <c r="G46" s="76"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="72"/>
+      <c r="G46" s="77"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A47" s="66">
+      <c r="A47" s="69">
         <v>3.4</v>
       </c>
       <c r="B47" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="77"/>
-      <c r="G47" s="76"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="72"/>
+      <c r="G47" s="77"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A48" s="66"/>
+      <c r="A48" s="69"/>
       <c r="B48" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="70"/>
-      <c r="D48" s="77"/>
-      <c r="G48" s="76"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="72"/>
+      <c r="G48" s="77"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A49" s="66"/>
+      <c r="A49" s="69"/>
       <c r="B49" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="70"/>
-      <c r="D49" s="77"/>
-      <c r="G49" s="76"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="72"/>
+      <c r="G49" s="77"/>
     </row>
     <row r="50" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="17">
@@ -3920,150 +3923,150 @@
       <c r="B50" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="71" t="s">
         <v>156</v>
       </c>
-      <c r="D50" s="77">
+      <c r="D50" s="72">
         <v>1</v>
       </c>
       <c r="E50" s="8"/>
-      <c r="G50" s="71" t="s">
+      <c r="G50" s="74" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A51" s="66">
+      <c r="A51" s="69">
         <v>4.0999999999999996</v>
       </c>
       <c r="B51" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="77"/>
-      <c r="G51" s="71"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="72"/>
+      <c r="G51" s="74"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A52" s="66"/>
+      <c r="A52" s="69"/>
       <c r="B52" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="70"/>
-      <c r="D52" s="77"/>
-      <c r="G52" s="71"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
+      <c r="G52" s="74"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A53" s="66"/>
+      <c r="A53" s="69"/>
       <c r="B53" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="70"/>
-      <c r="D53" s="77"/>
-      <c r="G53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="72"/>
+      <c r="G53" s="74"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A54" s="66"/>
+      <c r="A54" s="69"/>
       <c r="B54" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="70"/>
-      <c r="D54" s="77"/>
-      <c r="G54" s="71"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="72"/>
+      <c r="G54" s="74"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A55" s="66">
+      <c r="A55" s="69">
         <v>4.2</v>
       </c>
       <c r="B55" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="70"/>
-      <c r="D55" s="77"/>
-      <c r="G55" s="71"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="72"/>
+      <c r="G55" s="74"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A56" s="66"/>
+      <c r="A56" s="69"/>
       <c r="B56" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="70"/>
-      <c r="D56" s="77"/>
-      <c r="G56" s="71"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="72"/>
+      <c r="G56" s="74"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A57" s="66"/>
+      <c r="A57" s="69"/>
       <c r="B57" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="70"/>
-      <c r="D57" s="77"/>
-      <c r="G57" s="71"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="72"/>
+      <c r="G57" s="74"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A58" s="66">
+      <c r="A58" s="69">
         <v>4.3</v>
       </c>
       <c r="B58" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="70"/>
-      <c r="D58" s="77"/>
-      <c r="G58" s="71"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="72"/>
+      <c r="G58" s="74"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A59" s="66"/>
+      <c r="A59" s="69"/>
       <c r="B59" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="70"/>
-      <c r="D59" s="77"/>
-      <c r="G59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="72"/>
+      <c r="G59" s="74"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A60" s="66"/>
+      <c r="A60" s="69"/>
       <c r="B60" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="70"/>
-      <c r="D60" s="77"/>
-      <c r="G60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="72"/>
+      <c r="G60" s="74"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A61" s="66">
+      <c r="A61" s="69">
         <v>4.4000000000000004</v>
       </c>
       <c r="B61" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="70"/>
-      <c r="D61" s="77"/>
-      <c r="G61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="72"/>
+      <c r="G61" s="74"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A62" s="66"/>
+      <c r="A62" s="69"/>
       <c r="B62" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="70"/>
-      <c r="D62" s="77"/>
-      <c r="G62" s="71"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="72"/>
+      <c r="G62" s="74"/>
     </row>
     <row r="63" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="66"/>
+      <c r="A63" s="69"/>
       <c r="B63" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="70"/>
-      <c r="D63" s="77"/>
-      <c r="G63" s="71"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="72"/>
+      <c r="G63" s="74"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A64" s="66"/>
+      <c r="A64" s="69"/>
       <c r="B64" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="70"/>
-      <c r="D64" s="77"/>
-      <c r="G64" s="71"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="72"/>
+      <c r="G64" s="74"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A65" s="17">
@@ -4072,125 +4075,125 @@
       <c r="B65" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="70"/>
-      <c r="D65" s="77"/>
-      <c r="G65" s="71"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="72"/>
+      <c r="G65" s="74"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A66" s="66">
+      <c r="A66" s="69">
         <v>5.0999999999999996</v>
       </c>
       <c r="B66" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="70"/>
-      <c r="D66" s="77"/>
-      <c r="G66" s="71"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="72"/>
+      <c r="G66" s="74"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A67" s="66"/>
+      <c r="A67" s="69"/>
       <c r="B67" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="70"/>
-      <c r="D67" s="77"/>
-      <c r="G67" s="71"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="72"/>
+      <c r="G67" s="74"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A68" s="66"/>
+      <c r="A68" s="69"/>
       <c r="B68" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="70"/>
-      <c r="D68" s="77"/>
-      <c r="G68" s="71"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="72"/>
+      <c r="G68" s="74"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A69" s="66">
+      <c r="A69" s="69">
         <v>5.2</v>
       </c>
       <c r="B69" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="70"/>
-      <c r="D69" s="77"/>
-      <c r="G69" s="71"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="72"/>
+      <c r="G69" s="74"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A70" s="66"/>
+      <c r="A70" s="69"/>
       <c r="B70" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="70"/>
-      <c r="D70" s="77"/>
-      <c r="G70" s="71"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="72"/>
+      <c r="G70" s="74"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A71" s="66"/>
+      <c r="A71" s="69"/>
       <c r="B71" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="70"/>
-      <c r="D71" s="77"/>
-      <c r="G71" s="71"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="72"/>
+      <c r="G71" s="74"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A72" s="66">
+      <c r="A72" s="69">
         <v>5.3</v>
       </c>
       <c r="B72" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="C72" s="70"/>
-      <c r="D72" s="77"/>
-      <c r="G72" s="71"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="72"/>
+      <c r="G72" s="74"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A73" s="66"/>
+      <c r="A73" s="69"/>
       <c r="B73" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="70"/>
-      <c r="D73" s="77"/>
-      <c r="G73" s="71"/>
+      <c r="C73" s="71"/>
+      <c r="D73" s="72"/>
+      <c r="G73" s="74"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A74" s="66"/>
+      <c r="A74" s="69"/>
       <c r="B74" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="70"/>
-      <c r="D74" s="77"/>
-      <c r="G74" s="71"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="72"/>
+      <c r="G74" s="74"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A75" s="66">
+      <c r="A75" s="69">
         <v>5.4</v>
       </c>
       <c r="B75" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="70"/>
-      <c r="D75" s="77"/>
-      <c r="G75" s="71"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="72"/>
+      <c r="G75" s="74"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A76" s="66"/>
+      <c r="A76" s="69"/>
       <c r="B76" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="70"/>
-      <c r="D76" s="77"/>
-      <c r="G76" s="71"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="72"/>
+      <c r="G76" s="74"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A77" s="66"/>
+      <c r="A77" s="69"/>
       <c r="B77" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="70"/>
-      <c r="D77" s="77"/>
-      <c r="G77" s="71"/>
+      <c r="C77" s="71"/>
+      <c r="D77" s="72"/>
+      <c r="G77" s="74"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A78" s="17">
@@ -4199,199 +4202,199 @@
       <c r="B78" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="70"/>
-      <c r="D78" s="77"/>
-      <c r="G78" s="71"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="72"/>
+      <c r="G78" s="74"/>
     </row>
     <row r="79" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A79" s="68">
+      <c r="A79" s="73">
         <v>6.1</v>
       </c>
       <c r="B79" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="70"/>
-      <c r="D79" s="77"/>
-      <c r="G79" s="71"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="72"/>
+      <c r="G79" s="74"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A80" s="68"/>
+      <c r="A80" s="73"/>
       <c r="B80" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="70"/>
-      <c r="D80" s="77"/>
-      <c r="G80" s="71"/>
+      <c r="C80" s="71"/>
+      <c r="D80" s="72"/>
+      <c r="G80" s="74"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A81" s="68"/>
+      <c r="A81" s="73"/>
       <c r="B81" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="70"/>
-      <c r="D81" s="77"/>
-      <c r="G81" s="71"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="72"/>
+      <c r="G81" s="74"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A82" s="68"/>
+      <c r="A82" s="73"/>
       <c r="B82" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="70"/>
-      <c r="D82" s="77"/>
-      <c r="G82" s="71"/>
+      <c r="C82" s="71"/>
+      <c r="D82" s="72"/>
+      <c r="G82" s="74"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A83" s="68"/>
+      <c r="A83" s="73"/>
       <c r="B83" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="70"/>
-      <c r="D83" s="77"/>
-      <c r="G83" s="71"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="72"/>
+      <c r="G83" s="74"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A84" s="66">
+      <c r="A84" s="69">
         <v>6.2</v>
       </c>
       <c r="B84" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="70"/>
-      <c r="D84" s="77"/>
-      <c r="G84" s="71"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="72"/>
+      <c r="G84" s="74"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A85" s="66"/>
+      <c r="A85" s="69"/>
       <c r="B85" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C85" s="70"/>
-      <c r="D85" s="77"/>
-      <c r="G85" s="71"/>
+      <c r="C85" s="71"/>
+      <c r="D85" s="72"/>
+      <c r="G85" s="74"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A86" s="66"/>
+      <c r="A86" s="69"/>
       <c r="B86" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="70"/>
-      <c r="D86" s="77"/>
-      <c r="G86" s="71"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="72"/>
+      <c r="G86" s="74"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A87" s="66"/>
+      <c r="A87" s="69"/>
       <c r="B87" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="70"/>
-      <c r="D87" s="77"/>
-      <c r="G87" s="71"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="72"/>
+      <c r="G87" s="74"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A88" s="66"/>
+      <c r="A88" s="69"/>
       <c r="B88" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="70"/>
-      <c r="D88" s="77"/>
-      <c r="G88" s="71"/>
+      <c r="C88" s="71"/>
+      <c r="D88" s="72"/>
+      <c r="G88" s="74"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A89" s="66">
+      <c r="A89" s="69">
         <v>6.3</v>
       </c>
       <c r="B89" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C89" s="70"/>
-      <c r="D89" s="77"/>
-      <c r="G89" s="71"/>
+      <c r="C89" s="71"/>
+      <c r="D89" s="72"/>
+      <c r="G89" s="74"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A90" s="66"/>
+      <c r="A90" s="69"/>
       <c r="B90" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="70"/>
-      <c r="D90" s="77"/>
-      <c r="G90" s="71"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="72"/>
+      <c r="G90" s="74"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A91" s="66"/>
+      <c r="A91" s="69"/>
       <c r="B91" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C91" s="70"/>
-      <c r="D91" s="77"/>
-      <c r="G91" s="71"/>
+      <c r="C91" s="71"/>
+      <c r="D91" s="72"/>
+      <c r="G91" s="74"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A92" s="66">
+      <c r="A92" s="69">
         <v>6.4</v>
       </c>
       <c r="B92" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="70"/>
-      <c r="D92" s="77"/>
-      <c r="G92" s="71"/>
+      <c r="C92" s="71"/>
+      <c r="D92" s="72"/>
+      <c r="G92" s="74"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A93" s="66"/>
+      <c r="A93" s="69"/>
       <c r="B93" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="70"/>
-      <c r="D93" s="77"/>
-      <c r="G93" s="71"/>
+      <c r="C93" s="71"/>
+      <c r="D93" s="72"/>
+      <c r="G93" s="74"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A94" s="66"/>
+      <c r="A94" s="69"/>
       <c r="B94" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C94" s="70"/>
-      <c r="D94" s="77"/>
-      <c r="G94" s="71"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="72"/>
+      <c r="G94" s="74"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A95" s="66">
+      <c r="A95" s="69">
         <v>6.5</v>
       </c>
       <c r="B95" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C95" s="70"/>
-      <c r="D95" s="77"/>
-      <c r="G95" s="71"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="72"/>
+      <c r="G95" s="74"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A96" s="66"/>
+      <c r="A96" s="69"/>
       <c r="B96" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="70"/>
-      <c r="D96" s="77"/>
-      <c r="G96" s="71"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="72"/>
+      <c r="G96" s="74"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A97" s="66"/>
+      <c r="A97" s="69"/>
       <c r="B97" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="C97" s="70"/>
-      <c r="D97" s="77"/>
-      <c r="G97" s="71"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="72"/>
+      <c r="G97" s="74"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A98" s="66"/>
+      <c r="A98" s="69"/>
       <c r="B98" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="C98" s="70"/>
-      <c r="D98" s="77"/>
-      <c r="G98" s="71"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="72"/>
+      <c r="G98" s="74"/>
     </row>
     <row r="99" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A99" s="17">
@@ -4400,132 +4403,132 @@
       <c r="B99" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="D99" s="67">
+      <c r="D99" s="79">
         <v>1</v>
       </c>
       <c r="E99" s="8"/>
-      <c r="G99" s="69" t="s">
+      <c r="G99" s="82" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A100" s="66">
+      <c r="A100" s="69">
         <v>7.1</v>
       </c>
       <c r="B100" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="73"/>
-      <c r="D100" s="67"/>
-      <c r="G100" s="69"/>
+      <c r="C100" s="75"/>
+      <c r="D100" s="79"/>
+      <c r="G100" s="78"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A101" s="66"/>
+      <c r="A101" s="69"/>
       <c r="B101" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="73"/>
-      <c r="D101" s="67"/>
-      <c r="G101" s="69"/>
+      <c r="C101" s="75"/>
+      <c r="D101" s="79"/>
+      <c r="G101" s="78"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A102" s="66"/>
+      <c r="A102" s="69"/>
       <c r="B102" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="73"/>
-      <c r="D102" s="67"/>
-      <c r="G102" s="69"/>
+      <c r="C102" s="75"/>
+      <c r="D102" s="79"/>
+      <c r="G102" s="78"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A103" s="66">
+      <c r="A103" s="69">
         <v>7.2</v>
       </c>
       <c r="B103" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="73"/>
-      <c r="D103" s="67"/>
-      <c r="G103" s="69"/>
+      <c r="C103" s="75"/>
+      <c r="D103" s="79"/>
+      <c r="G103" s="78"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A104" s="66"/>
+      <c r="A104" s="69"/>
       <c r="B104" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="73"/>
-      <c r="D104" s="67"/>
-      <c r="G104" s="69"/>
+      <c r="C104" s="75"/>
+      <c r="D104" s="79"/>
+      <c r="G104" s="78"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A105" s="66"/>
+      <c r="A105" s="69"/>
       <c r="B105" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="73"/>
-      <c r="D105" s="67"/>
-      <c r="G105" s="69"/>
+      <c r="C105" s="75"/>
+      <c r="D105" s="79"/>
+      <c r="G105" s="78"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A106" s="66">
+      <c r="A106" s="69">
         <v>7.3</v>
       </c>
       <c r="B106" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="73"/>
-      <c r="D106" s="67"/>
-      <c r="G106" s="69"/>
+      <c r="C106" s="75"/>
+      <c r="D106" s="79"/>
+      <c r="G106" s="78"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A107" s="66"/>
+      <c r="A107" s="69"/>
       <c r="B107" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C107" s="73"/>
-      <c r="D107" s="67"/>
-      <c r="G107" s="69"/>
+      <c r="C107" s="75"/>
+      <c r="D107" s="79"/>
+      <c r="G107" s="78"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A108" s="66"/>
+      <c r="A108" s="69"/>
       <c r="B108" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="73"/>
-      <c r="D108" s="67"/>
-      <c r="G108" s="69"/>
+      <c r="C108" s="75"/>
+      <c r="D108" s="79"/>
+      <c r="G108" s="78"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A109" s="66">
+      <c r="A109" s="69">
         <v>7.4</v>
       </c>
       <c r="B109" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="73"/>
-      <c r="D109" s="67"/>
-      <c r="G109" s="69"/>
+      <c r="C109" s="75"/>
+      <c r="D109" s="79"/>
+      <c r="G109" s="78"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A110" s="66"/>
+      <c r="A110" s="69"/>
       <c r="B110" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="73"/>
-      <c r="D110" s="67"/>
-      <c r="G110" s="69"/>
+      <c r="C110" s="75"/>
+      <c r="D110" s="79"/>
+      <c r="G110" s="78"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A111" s="66"/>
+      <c r="A111" s="69"/>
       <c r="B111" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C111" s="73"/>
-      <c r="D111" s="67"/>
-      <c r="G111" s="69"/>
+      <c r="C111" s="75"/>
+      <c r="D111" s="79"/>
+      <c r="G111" s="78"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A112" s="21">
@@ -4534,9 +4537,9 @@
       <c r="B112" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C112" s="73"/>
-      <c r="D112" s="67"/>
-      <c r="G112" s="69"/>
+      <c r="C112" s="75"/>
+      <c r="D112" s="79"/>
+      <c r="G112" s="78"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A113" s="21">
@@ -4545,101 +4548,101 @@
       <c r="B113" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="73"/>
-      <c r="D113" s="67"/>
-      <c r="G113" s="69"/>
+      <c r="C113" s="75"/>
+      <c r="D113" s="79"/>
+      <c r="G113" s="78"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A114" s="66">
+      <c r="A114" s="69">
         <v>8.1</v>
       </c>
       <c r="B114" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C114" s="73"/>
-      <c r="D114" s="67"/>
-      <c r="G114" s="69"/>
+      <c r="C114" s="75"/>
+      <c r="D114" s="79"/>
+      <c r="G114" s="78"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A115" s="66"/>
+      <c r="A115" s="69"/>
       <c r="B115" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="C115" s="73"/>
-      <c r="D115" s="67"/>
-      <c r="G115" s="69"/>
+      <c r="C115" s="75"/>
+      <c r="D115" s="79"/>
+      <c r="G115" s="78"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A116" s="66"/>
-      <c r="B116" s="79" t="s">
+      <c r="A116" s="69"/>
+      <c r="B116" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C116" s="73"/>
-      <c r="D116" s="67"/>
-      <c r="G116" s="69"/>
+      <c r="C116" s="75"/>
+      <c r="D116" s="79"/>
+      <c r="G116" s="78"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A117" s="66"/>
-      <c r="B117" s="79" t="s">
+      <c r="A117" s="69"/>
+      <c r="B117" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C117" s="73"/>
-      <c r="D117" s="67"/>
-      <c r="G117" s="69"/>
+      <c r="C117" s="75"/>
+      <c r="D117" s="79"/>
+      <c r="G117" s="78"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A118" s="66"/>
-      <c r="B118" s="79" t="s">
+      <c r="A118" s="69"/>
+      <c r="B118" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="C118" s="73"/>
-      <c r="D118" s="67"/>
-      <c r="G118" s="69"/>
+      <c r="C118" s="75"/>
+      <c r="D118" s="79"/>
+      <c r="G118" s="78"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A119" s="66"/>
-      <c r="B119" s="79" t="s">
+      <c r="A119" s="69"/>
+      <c r="B119" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="C119" s="73"/>
-      <c r="D119" s="67"/>
-      <c r="G119" s="69"/>
+      <c r="C119" s="75"/>
+      <c r="D119" s="79"/>
+      <c r="G119" s="78"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A120" s="66"/>
-      <c r="B120" s="80" t="s">
+      <c r="A120" s="69"/>
+      <c r="B120" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="C120" s="73"/>
-      <c r="D120" s="67"/>
-      <c r="G120" s="69"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="79"/>
+      <c r="G120" s="78"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A121" s="66"/>
-      <c r="B121" s="80" t="s">
+      <c r="A121" s="69"/>
+      <c r="B121" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="C121" s="73"/>
-      <c r="D121" s="67"/>
-      <c r="G121" s="69"/>
+      <c r="C121" s="75"/>
+      <c r="D121" s="79"/>
+      <c r="G121" s="78"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A122" s="66"/>
+      <c r="A122" s="69"/>
       <c r="B122" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="C122" s="73"/>
-      <c r="D122" s="67"/>
-      <c r="G122" s="69"/>
+      <c r="C122" s="75"/>
+      <c r="D122" s="79"/>
+      <c r="G122" s="78"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A123" s="66"/>
+      <c r="A123" s="69"/>
       <c r="B123" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="C123" s="73"/>
-      <c r="D123" s="67"/>
-      <c r="G123" s="69"/>
+      <c r="C123" s="75"/>
+      <c r="D123" s="79"/>
+      <c r="G123" s="78"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A124" s="17">
@@ -4648,175 +4651,175 @@
       <c r="B124" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C124" s="73" t="s">
+      <c r="C124" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="D124" s="67">
+      <c r="D124" s="79">
         <v>0.75</v>
       </c>
       <c r="E124" s="8"/>
-      <c r="G124" s="69"/>
+      <c r="G124" s="78"/>
     </row>
     <row r="125" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A125" s="68">
+      <c r="A125" s="73">
         <v>9.1</v>
       </c>
       <c r="B125" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C125" s="73"/>
-      <c r="D125" s="67"/>
-      <c r="G125" s="69"/>
+      <c r="C125" s="75"/>
+      <c r="D125" s="79"/>
+      <c r="G125" s="78"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A126" s="68"/>
+      <c r="A126" s="73"/>
       <c r="B126" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C126" s="73"/>
-      <c r="D126" s="67"/>
-      <c r="G126" s="69"/>
+      <c r="C126" s="75"/>
+      <c r="D126" s="79"/>
+      <c r="G126" s="78"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A127" s="68"/>
+      <c r="A127" s="73"/>
       <c r="B127" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C127" s="73"/>
-      <c r="D127" s="67"/>
-      <c r="G127" s="69"/>
+      <c r="C127" s="75"/>
+      <c r="D127" s="79"/>
+      <c r="G127" s="78"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A128" s="68"/>
+      <c r="A128" s="73"/>
       <c r="B128" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C128" s="73"/>
-      <c r="D128" s="67"/>
-      <c r="G128" s="69"/>
+      <c r="C128" s="75"/>
+      <c r="D128" s="79"/>
+      <c r="G128" s="78"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A129" s="68"/>
+      <c r="A129" s="73"/>
       <c r="B129" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C129" s="73"/>
-      <c r="D129" s="67"/>
-      <c r="G129" s="69"/>
+      <c r="C129" s="75"/>
+      <c r="D129" s="79"/>
+      <c r="G129" s="78"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A130" s="66">
+      <c r="A130" s="69">
         <v>9.1999999999999993</v>
       </c>
       <c r="B130" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C130" s="73"/>
-      <c r="D130" s="67"/>
-      <c r="G130" s="69"/>
+      <c r="C130" s="75"/>
+      <c r="D130" s="79"/>
+      <c r="G130" s="78"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A131" s="66"/>
+      <c r="A131" s="69"/>
       <c r="B131" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C131" s="73"/>
-      <c r="D131" s="67"/>
-      <c r="G131" s="69"/>
+      <c r="C131" s="75"/>
+      <c r="D131" s="79"/>
+      <c r="G131" s="78"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A132" s="66"/>
+      <c r="A132" s="69"/>
       <c r="B132" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C132" s="73"/>
-      <c r="D132" s="67"/>
-      <c r="G132" s="69"/>
+      <c r="C132" s="75"/>
+      <c r="D132" s="79"/>
+      <c r="G132" s="78"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A133" s="66"/>
+      <c r="A133" s="69"/>
       <c r="B133" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C133" s="73"/>
-      <c r="D133" s="67"/>
-      <c r="G133" s="69"/>
+      <c r="C133" s="75"/>
+      <c r="D133" s="79"/>
+      <c r="G133" s="78"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A134" s="66">
+      <c r="A134" s="69">
         <v>9.3000000000000007</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C134" s="73"/>
-      <c r="D134" s="67"/>
-      <c r="G134" s="69"/>
+      <c r="C134" s="75"/>
+      <c r="D134" s="79"/>
+      <c r="G134" s="78"/>
     </row>
     <row r="135" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A135" s="66"/>
+      <c r="A135" s="69"/>
       <c r="B135" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C135" s="73"/>
-      <c r="D135" s="67"/>
-      <c r="G135" s="69"/>
+      <c r="C135" s="75"/>
+      <c r="D135" s="79"/>
+      <c r="G135" s="78"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A136" s="66"/>
+      <c r="A136" s="69"/>
       <c r="B136" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C136" s="73"/>
-      <c r="D136" s="67"/>
-      <c r="G136" s="69"/>
+      <c r="C136" s="75"/>
+      <c r="D136" s="79"/>
+      <c r="G136" s="78"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A137" s="66"/>
+      <c r="A137" s="69"/>
       <c r="B137" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C137" s="73"/>
-      <c r="D137" s="67"/>
-      <c r="G137" s="69"/>
+      <c r="C137" s="75"/>
+      <c r="D137" s="79"/>
+      <c r="G137" s="78"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A138" s="66">
+      <c r="A138" s="69">
         <v>9.4</v>
       </c>
       <c r="B138" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C138" s="73"/>
-      <c r="D138" s="67"/>
-      <c r="G138" s="69"/>
+      <c r="C138" s="75"/>
+      <c r="D138" s="79"/>
+      <c r="G138" s="78"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A139" s="66"/>
+      <c r="A139" s="69"/>
       <c r="B139" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C139" s="73"/>
-      <c r="D139" s="67"/>
-      <c r="G139" s="69"/>
+      <c r="C139" s="75"/>
+      <c r="D139" s="79"/>
+      <c r="G139" s="78"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A140" s="66"/>
+      <c r="A140" s="69"/>
       <c r="B140" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C140" s="73"/>
-      <c r="D140" s="67"/>
-      <c r="G140" s="69"/>
+      <c r="C140" s="75"/>
+      <c r="D140" s="79"/>
+      <c r="G140" s="78"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A141" s="66"/>
+      <c r="A141" s="69"/>
       <c r="B141" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C141" s="73"/>
-      <c r="D141" s="67"/>
-      <c r="G141" s="69"/>
+      <c r="C141" s="75"/>
+      <c r="D141" s="79"/>
+      <c r="G141" s="78"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A142" s="17">
@@ -4825,25 +4828,25 @@
       <c r="B142" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="70" t="s">
+      <c r="C142" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="D142" s="67">
+      <c r="D142" s="79">
         <v>1.75</v>
       </c>
       <c r="E142" s="8"/>
-      <c r="G142" s="69"/>
+      <c r="G142" s="78"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A143" s="21">
         <v>10.1</v>
       </c>
-      <c r="B143" s="81" t="s">
+      <c r="B143" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="70"/>
-      <c r="D143" s="67"/>
-      <c r="G143" s="69"/>
+      <c r="C143" s="71"/>
+      <c r="D143" s="79"/>
+      <c r="G143" s="78"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.6">
       <c r="A144" s="17">
@@ -4852,180 +4855,222 @@
       <c r="B144" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C144" s="73" t="s">
+      <c r="C144" s="75" t="s">
         <v>169</v>
       </c>
-      <c r="D144" s="67">
+      <c r="D144" s="79">
         <v>0.5</v>
       </c>
       <c r="E144" s="8"/>
-      <c r="G144" s="71"/>
+      <c r="G144" s="74"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A145" s="66">
+      <c r="A145" s="69">
         <v>11.1</v>
       </c>
       <c r="B145" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C145" s="74"/>
-      <c r="D145" s="67"/>
-      <c r="G145" s="71"/>
+      <c r="C145" s="81"/>
+      <c r="D145" s="79"/>
+      <c r="G145" s="74"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A146" s="66"/>
+      <c r="A146" s="69"/>
       <c r="B146" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C146" s="74"/>
-      <c r="D146" s="67"/>
-      <c r="G146" s="71"/>
+      <c r="C146" s="81"/>
+      <c r="D146" s="79"/>
+      <c r="G146" s="74"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A147" s="66"/>
+      <c r="A147" s="69"/>
       <c r="B147" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C147" s="74"/>
-      <c r="D147" s="67"/>
-      <c r="G147" s="71"/>
+      <c r="C147" s="81"/>
+      <c r="D147" s="79"/>
+      <c r="G147" s="74"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A148" s="66">
+      <c r="A148" s="69">
         <v>11.2</v>
       </c>
       <c r="B148" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C148" s="74"/>
-      <c r="D148" s="67"/>
-      <c r="G148" s="71"/>
+      <c r="C148" s="81"/>
+      <c r="D148" s="79"/>
+      <c r="G148" s="74"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A149" s="66"/>
+      <c r="A149" s="69"/>
       <c r="B149" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C149" s="74"/>
-      <c r="D149" s="67"/>
-      <c r="G149" s="71"/>
+      <c r="C149" s="81"/>
+      <c r="D149" s="79"/>
+      <c r="G149" s="74"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A150" s="66"/>
+      <c r="A150" s="69"/>
       <c r="B150" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C150" s="74"/>
-      <c r="D150" s="67"/>
-      <c r="G150" s="71"/>
+      <c r="C150" s="81"/>
+      <c r="D150" s="79"/>
+      <c r="G150" s="74"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A151" s="72">
+      <c r="A151" s="80">
         <v>11.3</v>
       </c>
       <c r="B151" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C151" s="74"/>
-      <c r="D151" s="67"/>
-      <c r="G151" s="71"/>
+      <c r="C151" s="81"/>
+      <c r="D151" s="79"/>
+      <c r="G151" s="74"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A152" s="72"/>
+      <c r="A152" s="80"/>
       <c r="B152" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="74"/>
-      <c r="D152" s="67"/>
-      <c r="G152" s="71"/>
+      <c r="C152" s="81"/>
+      <c r="D152" s="79"/>
+      <c r="G152" s="74"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A153" s="72"/>
+      <c r="A153" s="80"/>
       <c r="B153" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C153" s="74"/>
-      <c r="D153" s="67"/>
-      <c r="G153" s="71"/>
+      <c r="C153" s="81"/>
+      <c r="D153" s="79"/>
+      <c r="G153" s="74"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A154" s="72"/>
+      <c r="A154" s="80"/>
       <c r="B154" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C154" s="74"/>
-      <c r="D154" s="67"/>
-      <c r="G154" s="71"/>
+      <c r="C154" s="81"/>
+      <c r="D154" s="79"/>
+      <c r="G154" s="74"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A155" s="72">
+      <c r="A155" s="80">
         <v>11.4</v>
       </c>
       <c r="B155" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C155" s="74"/>
-      <c r="D155" s="67"/>
-      <c r="G155" s="71"/>
+      <c r="C155" s="81"/>
+      <c r="D155" s="79"/>
+      <c r="G155" s="74"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A156" s="72"/>
+      <c r="A156" s="80"/>
       <c r="B156" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C156" s="74"/>
-      <c r="D156" s="67"/>
-      <c r="G156" s="71"/>
+      <c r="C156" s="81"/>
+      <c r="D156" s="79"/>
+      <c r="G156" s="74"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A157" s="72"/>
+      <c r="A157" s="80"/>
       <c r="B157" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C157" s="74"/>
-      <c r="D157" s="67"/>
-      <c r="G157" s="71"/>
+      <c r="C157" s="81"/>
+      <c r="D157" s="79"/>
+      <c r="G157" s="74"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A158" s="72">
+      <c r="A158" s="80">
         <v>11.5</v>
       </c>
       <c r="B158" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C158" s="74"/>
-      <c r="D158" s="67"/>
-      <c r="G158" s="71"/>
+      <c r="C158" s="81"/>
+      <c r="D158" s="79"/>
+      <c r="G158" s="74"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A159" s="72"/>
+      <c r="A159" s="80"/>
       <c r="B159" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="C159" s="74"/>
-      <c r="D159" s="67"/>
-      <c r="G159" s="71"/>
+      <c r="C159" s="81"/>
+      <c r="D159" s="79"/>
+      <c r="G159" s="74"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A160" s="72"/>
+      <c r="A160" s="80"/>
       <c r="B160" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C160" s="74"/>
-      <c r="D160" s="67"/>
-      <c r="G160" s="71"/>
+      <c r="C160" s="81"/>
+      <c r="D160" s="79"/>
+      <c r="G160" s="74"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A161" s="72"/>
+      <c r="A161" s="80"/>
       <c r="B161" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C161" s="74"/>
-      <c r="D161" s="67"/>
-      <c r="G161" s="71"/>
+      <c r="C161" s="81"/>
+      <c r="D161" s="79"/>
+      <c r="G161" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="D124:D141"/>
+    <mergeCell ref="A125:A129"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="G144:G161"/>
+    <mergeCell ref="D144:D161"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="A158:A161"/>
+    <mergeCell ref="C144:C161"/>
+    <mergeCell ref="C99:C123"/>
+    <mergeCell ref="G5:G49"/>
+    <mergeCell ref="G99:G141"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="C124:C141"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="D99:D123"/>
+    <mergeCell ref="C50:C98"/>
+    <mergeCell ref="D50:D98"/>
+    <mergeCell ref="G50:G98"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A95:A98"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="C5:C49"/>
@@ -5042,48 +5087,6 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C50:C98"/>
-    <mergeCell ref="D50:D98"/>
-    <mergeCell ref="G50:G98"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="C99:C123"/>
-    <mergeCell ref="G5:G49"/>
-    <mergeCell ref="G99:G141"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="C124:C141"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="D99:D123"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="G144:G161"/>
-    <mergeCell ref="D144:D161"/>
-    <mergeCell ref="A148:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A155:A157"/>
-    <mergeCell ref="A158:A161"/>
-    <mergeCell ref="C144:C161"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="A138:A141"/>
-    <mergeCell ref="D124:D141"/>
-    <mergeCell ref="A125:A129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>